<commit_message>
Updated rho distribution scale parameter value and value for parameters for age of first reproduction. Corrects bugs and updates analysis.
</commit_message>
<xml_diff>
--- a/FolderArchitecture2runCode/InputFiles/SpeciesDefinitionFile.xlsx
+++ b/FolderArchitecture2runCode/InputFiles/SpeciesDefinitionFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tam2\Dropbox\Trabalho\Funded\CARMMHA\integrativemodelling\FinalModelRuns\CARMMHAgit\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBD3A5A-878C-44EA-B40A-277B036A2DE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F5D681-A8A1-4036-838B-3401BBDAF007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51720" yWindow="-3015" windowWidth="51840" windowHeight="21240" tabRatio="930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="values" sheetId="32" r:id="rId1"/>
@@ -35,7 +35,6 @@
   <authors>
     <author>tc={B9B7C426-47BA-4521-B1F7-2A389A2A4367}</author>
     <author>tc={CD5CF19A-9F60-4FEE-8330-A3BF39F0CD02}</author>
-    <author>tc={F76610AF-C3F2-43AB-BA41-A8DE405A3B72}</author>
     <author>tc={CA68C946-F89E-42BB-BC70-9CA308F156BC}</author>
     <author>tc={FBDD81FD-7A18-4735-8879-CB35D02C7391}</author>
     <author>tc={9555694C-6EFE-4219-8D3C-BBE6F63D7731}</author>
@@ -59,24 +58,7 @@
     value changed from 0.34 on the 21st April 2021. See email from Len Mon 4/19/2021 12:15 AM replying to Lori (Sun 4/18/2021 10:18 PM)</t>
       </text>
     </comment>
-    <comment ref="C25" authorId="2" shapeId="0" xr:uid="{F76610AF-C3F2-43AB-BA41-A8DE405A3B72}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    #we want this mean and sd
-mean=7.52
-sd=0.274
-sha=(mean^2)/(sd^2)
-sca=(sd^2)/(mean)
-based on 
-Fecundity-related parameters in the bottlenose dolphin population model.
-Len Thomas
-Last compiled on 20 June, 2020
-see also Age1stRepPars.R</t>
-      </text>
-    </comment>
-    <comment ref="W25" authorId="3" shapeId="0" xr:uid="{CA68C946-F89E-42BB-BC70-9CA308F156BC}">
+    <comment ref="W25" authorId="2" shapeId="0" xr:uid="{CA68C946-F89E-42BB-BC70-9CA308F156BC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -84,7 +66,7 @@
     value changed from 0.34 on the 21st April 2021. See email from Len Mon 4/19/2021 12:15 AM replying to Lori (Sun 4/18/2021 10:18 PM)</t>
       </text>
     </comment>
-    <comment ref="AA25" authorId="4" shapeId="0" xr:uid="{FBDD81FD-7A18-4735-8879-CB35D02C7391}">
+    <comment ref="AA25" authorId="3" shapeId="0" xr:uid="{FBDD81FD-7A18-4735-8879-CB35D02C7391}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -92,7 +74,7 @@
     will come from Richard's analysis</t>
       </text>
     </comment>
-    <comment ref="AO25" authorId="5" shapeId="0" xr:uid="{9555694C-6EFE-4219-8D3C-BBE6F63D7731}">
+    <comment ref="AO25" authorId="4" shapeId="0" xr:uid="{9555694C-6EFE-4219-8D3C-BBE6F63D7731}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -882,7 +864,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1023,12 +1005,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="43">
@@ -2083,18 +2059,6 @@
   <threadedComment ref="W18" dT="2021-04-21T11:53:29.42" personId="{43E54F80-8E8C-427E-A997-6277C6651A43}" id="{CD5CF19A-9F60-4FEE-8330-A3BF39F0CD02}">
     <text>value changed from 0.34 on the 21st April 2021. See email from Len Mon 4/19/2021 12:15 AM replying to Lori (Sun 4/18/2021 10:18 PM)</text>
   </threadedComment>
-  <threadedComment ref="C25" dT="2020-06-15T12:00:17.63" personId="{43E54F80-8E8C-427E-A997-6277C6651A43}" id="{F76610AF-C3F2-43AB-BA41-A8DE405A3B72}">
-    <text>#we want this mean and sd
-mean=7.52
-sd=0.274
-sha=(mean^2)/(sd^2)
-sca=(sd^2)/(mean)
-based on 
-Fecundity-related parameters in the bottlenose dolphin population model.
-Len Thomas
-Last compiled on 20 June, 2020
-see also Age1stRepPars.R</text>
-  </threadedComment>
   <threadedComment ref="W25" dT="2021-04-21T11:53:29.42" personId="{43E54F80-8E8C-427E-A997-6277C6651A43}" id="{CA68C946-F89E-42BB-BC70-9CA308F156BC}">
     <text>value changed from 0.34 on the 21st April 2021. See email from Len Mon 4/19/2021 12:15 AM replying to Lori (Sun 4/18/2021 10:18 PM)</text>
   </threadedComment>
@@ -2115,41 +2079,41 @@
   <dimension ref="A1:BG34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W25" sqref="W25"/>
+      <selection pane="bottomRight" activeCell="U36" sqref="U36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="8.77734375" style="4"/>
-    <col min="10" max="16" width="8.77734375" style="7"/>
-    <col min="17" max="17" width="8.77734375" style="4"/>
+    <col min="1" max="1" width="21.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="8.81640625" style="4"/>
+    <col min="10" max="16" width="8.81640625" style="7"/>
+    <col min="17" max="17" width="8.81640625" style="4"/>
     <col min="18" max="18" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="24" width="8.77734375" style="4"/>
-    <col min="25" max="25" width="9.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="45" width="8.77734375" style="4"/>
-    <col min="46" max="46" width="8.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="24" width="8.81640625" style="4"/>
+    <col min="25" max="25" width="9.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="45" width="8.81640625" style="4"/>
+    <col min="46" max="46" width="8.81640625" style="4" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="10.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="7.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="50" max="51" width="7.109375" style="4" customWidth="1"/>
-    <col min="52" max="52" width="7.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="7.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="50" max="51" width="7.08984375" style="4" customWidth="1"/>
+    <col min="52" max="52" width="7.81640625" style="4" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="4.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="29.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="35.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="36.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="30.77734375" style="4" customWidth="1"/>
-    <col min="59" max="59" width="27.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="60" max="16384" width="8.77734375" style="4"/>
+    <col min="54" max="54" width="4.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="29.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="35.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="36.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="30.81640625" style="4" customWidth="1"/>
+    <col min="59" max="59" width="27.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="60" max="16384" width="8.81640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -2328,7 +2292,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -2404,8 +2368,8 @@
       <c r="Y2" s="4">
         <v>6.34</v>
       </c>
-      <c r="Z2" s="4">
-        <v>0.85299999999999998</v>
+      <c r="Z2">
+        <v>1.1723330000000001</v>
       </c>
       <c r="AA2" s="7">
         <v>0.72</v>
@@ -2507,7 +2471,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>197</v>
       </c>
@@ -2583,8 +2547,8 @@
       <c r="Y3" s="4">
         <v>6.34</v>
       </c>
-      <c r="Z3" s="4">
-        <v>0.85299999999999998</v>
+      <c r="Z3" s="1">
+        <v>1.1723330000000001</v>
       </c>
       <c r="AA3" s="4">
         <v>0.63</v>
@@ -2683,7 +2647,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>44</v>
       </c>
@@ -2759,8 +2723,8 @@
       <c r="Y4" s="4">
         <v>6.34</v>
       </c>
-      <c r="Z4" s="4">
-        <v>0.85299999999999998</v>
+      <c r="Z4" s="1">
+        <v>1.1723330000000001</v>
       </c>
       <c r="AA4" s="4">
         <v>0.7</v>
@@ -2859,7 +2823,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>41</v>
       </c>
@@ -2935,8 +2899,8 @@
       <c r="Y5" s="4">
         <v>6.34</v>
       </c>
-      <c r="Z5" s="4">
-        <v>0.85299999999999998</v>
+      <c r="Z5" s="1">
+        <v>1.1723330000000001</v>
       </c>
       <c r="AA5" s="4">
         <v>0.7</v>
@@ -3035,7 +2999,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>246</v>
       </c>
@@ -3111,8 +3075,8 @@
       <c r="Y6" s="4">
         <v>6.34</v>
       </c>
-      <c r="Z6" s="4">
-        <v>0.85299999999999998</v>
+      <c r="Z6" s="1">
+        <v>1.1723330000000001</v>
       </c>
       <c r="AA6" s="4">
         <v>0.7</v>
@@ -3211,7 +3175,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>182</v>
       </c>
@@ -3287,8 +3251,8 @@
       <c r="Y7" s="4">
         <v>6.34</v>
       </c>
-      <c r="Z7" s="4">
-        <v>0.85299999999999998</v>
+      <c r="Z7" s="1">
+        <v>1.1723330000000001</v>
       </c>
       <c r="AA7" s="7">
         <v>0.7</v>
@@ -3390,7 +3354,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="8" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -3466,8 +3430,8 @@
       <c r="Y8" s="4">
         <v>6.34</v>
       </c>
-      <c r="Z8" s="4">
-        <v>0.85299999999999998</v>
+      <c r="Z8" s="1">
+        <v>1.1723330000000001</v>
       </c>
       <c r="AA8" s="7">
         <v>0.7</v>
@@ -3566,7 +3530,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>180</v>
       </c>
@@ -3642,8 +3606,8 @@
       <c r="Y9" s="4">
         <v>6.34</v>
       </c>
-      <c r="Z9" s="4">
-        <v>0.85299999999999998</v>
+      <c r="Z9" s="1">
+        <v>1.1723330000000001</v>
       </c>
       <c r="AA9" s="7">
         <v>0.7</v>
@@ -3745,7 +3709,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="10" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>181</v>
       </c>
@@ -3821,8 +3785,8 @@
       <c r="Y10" s="4">
         <v>6.34</v>
       </c>
-      <c r="Z10" s="4">
-        <v>0.85299999999999998</v>
+      <c r="Z10" s="1">
+        <v>1.1723330000000001</v>
       </c>
       <c r="AA10" s="4">
         <v>0.75</v>
@@ -3924,7 +3888,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>177</v>
       </c>
@@ -4000,8 +3964,8 @@
       <c r="Y11" s="4">
         <v>6.34</v>
       </c>
-      <c r="Z11" s="4">
-        <v>0.85299999999999998</v>
+      <c r="Z11" s="1">
+        <v>1.1723330000000001</v>
       </c>
       <c r="AA11" s="4">
         <v>0.63</v>
@@ -4103,7 +4067,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>178</v>
       </c>
@@ -4179,8 +4143,8 @@
       <c r="Y12" s="4">
         <v>6.34</v>
       </c>
-      <c r="Z12" s="4">
-        <v>0.85299999999999998</v>
+      <c r="Z12" s="1">
+        <v>1.1723330000000001</v>
       </c>
       <c r="AA12" s="4">
         <v>0.63</v>
@@ -4282,7 +4246,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="13" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>30</v>
       </c>
@@ -4358,8 +4322,8 @@
       <c r="Y13" s="4">
         <v>6.34</v>
       </c>
-      <c r="Z13" s="4">
-        <v>0.85299999999999998</v>
+      <c r="Z13" s="1">
+        <v>1.1723330000000001</v>
       </c>
       <c r="AA13" s="7">
         <v>0.7</v>
@@ -4461,7 +4425,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="14" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>31</v>
       </c>
@@ -4537,8 +4501,8 @@
       <c r="Y14" s="4">
         <v>6.34</v>
       </c>
-      <c r="Z14" s="4">
-        <v>0.85299999999999998</v>
+      <c r="Z14" s="1">
+        <v>1.1723330000000001</v>
       </c>
       <c r="AA14" s="7">
         <v>0.7</v>
@@ -4637,7 +4601,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>3</v>
       </c>
@@ -4713,8 +4677,8 @@
       <c r="Y15" s="4">
         <v>6.34</v>
       </c>
-      <c r="Z15" s="4">
-        <v>0.85299999999999998</v>
+      <c r="Z15" s="1">
+        <v>1.1723330000000001</v>
       </c>
       <c r="AA15" s="7">
         <v>0.63</v>
@@ -4813,7 +4777,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>54</v>
       </c>
@@ -4889,8 +4853,8 @@
       <c r="Y16" s="4">
         <v>6.34</v>
       </c>
-      <c r="Z16" s="4">
-        <v>0.85299999999999998</v>
+      <c r="Z16" s="1">
+        <v>1.1723330000000001</v>
       </c>
       <c r="AA16" s="4">
         <v>0.75</v>
@@ -4989,7 +4953,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="17" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>50</v>
       </c>
@@ -5065,8 +5029,8 @@
       <c r="Y17" s="4">
         <v>6.34</v>
       </c>
-      <c r="Z17" s="4">
-        <v>0.85299999999999998</v>
+      <c r="Z17" s="1">
+        <v>1.1723330000000001</v>
       </c>
       <c r="AA17" s="4">
         <v>0.7</v>
@@ -5165,7 +5129,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="18" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>189</v>
       </c>
@@ -5345,7 +5309,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="19" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>21</v>
       </c>
@@ -5421,8 +5385,8 @@
       <c r="Y19" s="4">
         <v>6.34</v>
       </c>
-      <c r="Z19" s="4">
-        <v>0.85299999999999998</v>
+      <c r="Z19">
+        <v>1.1723330000000001</v>
       </c>
       <c r="AA19" s="7">
         <v>0.75</v>
@@ -5521,7 +5485,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="20" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>64</v>
       </c>
@@ -5597,8 +5561,8 @@
       <c r="Y20" s="4">
         <v>6.34</v>
       </c>
-      <c r="Z20" s="4">
-        <v>0.85299999999999998</v>
+      <c r="Z20" s="1">
+        <v>1.1723330000000001</v>
       </c>
       <c r="AA20" s="4">
         <v>0.75</v>
@@ -5697,7 +5661,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="21" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>161</v>
       </c>
@@ -5773,8 +5737,8 @@
       <c r="Y21" s="4">
         <v>6.34</v>
       </c>
-      <c r="Z21" s="4">
-        <v>0.85299999999999998</v>
+      <c r="Z21" s="1">
+        <v>1.1723330000000001</v>
       </c>
       <c r="AA21" s="4">
         <v>0.75</v>
@@ -5873,7 +5837,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>65</v>
       </c>
@@ -5949,8 +5913,8 @@
       <c r="Y22" s="4">
         <v>6.34</v>
       </c>
-      <c r="Z22" s="4">
-        <v>0.85299999999999998</v>
+      <c r="Z22" s="1">
+        <v>1.1723330000000001</v>
       </c>
       <c r="AA22" s="4">
         <v>0.75</v>
@@ -6049,7 +6013,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="23" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>38</v>
       </c>
@@ -6125,8 +6089,8 @@
       <c r="Y23" s="4">
         <v>6.34</v>
       </c>
-      <c r="Z23" s="4">
-        <v>0.85299999999999998</v>
+      <c r="Z23" s="1">
+        <v>1.1723330000000001</v>
       </c>
       <c r="AA23" s="7">
         <v>0.7</v>
@@ -6225,7 +6189,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>57</v>
       </c>
@@ -6301,8 +6265,8 @@
       <c r="Y24" s="4">
         <v>6.34</v>
       </c>
-      <c r="Z24" s="4">
-        <v>0.85299999999999998</v>
+      <c r="Z24" s="1">
+        <v>1.1723330000000001</v>
       </c>
       <c r="AA24" s="4">
         <v>0.75</v>
@@ -6401,18 +6365,18 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>71</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C25" s="4">
-        <v>753.24199999999996</v>
-      </c>
-      <c r="D25" s="4">
-        <v>9.9835110000000005E-3</v>
+      <c r="C25">
+        <v>980.35320549999994</v>
+      </c>
+      <c r="D25">
+        <v>8.7495999999999997E-3</v>
       </c>
       <c r="E25" s="4">
         <v>48</v>
@@ -6477,8 +6441,8 @@
       <c r="Y25" s="4">
         <v>6.34</v>
       </c>
-      <c r="Z25" s="4">
-        <v>0.85299999999999998</v>
+      <c r="Z25" s="1">
+        <v>1.1723330000000001</v>
       </c>
       <c r="AA25" s="10">
         <v>0.7</v>
@@ -6577,7 +6541,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="26" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>179</v>
       </c>
@@ -6653,8 +6617,8 @@
       <c r="Y26" s="4">
         <v>6.34</v>
       </c>
-      <c r="Z26" s="4">
-        <v>0.85299999999999998</v>
+      <c r="Z26" s="1">
+        <v>1.1723330000000001</v>
       </c>
       <c r="AA26" s="4">
         <v>0.63</v>
@@ -6756,7 +6720,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:59" x14ac:dyDescent="0.35">
       <c r="AA27" s="7"/>
       <c r="AB27" s="7"/>
       <c r="AC27" s="7"/>
@@ -6765,10 +6729,10 @@
       <c r="AF27" s="7"/>
       <c r="BD27" s="7"/>
     </row>
-    <row r="28" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:59" x14ac:dyDescent="0.35">
       <c r="BD28" s="7"/>
     </row>
-    <row r="34" spans="18:33" x14ac:dyDescent="0.3">
+    <row r="34" spans="18:33" x14ac:dyDescent="0.35">
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
       <c r="T34" s="8"/>
@@ -6804,16 +6768,16 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="2" max="2" width="91.21875" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="93.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.08984375" customWidth="1"/>
+    <col min="2" max="2" width="91.1796875" customWidth="1"/>
+    <col min="3" max="3" width="25.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="93.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="92" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>90</v>
       </c>
@@ -6830,7 +6794,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6847,7 +6811,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -6864,7 +6828,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>159</v>
       </c>
@@ -6881,7 +6845,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>160</v>
       </c>
@@ -6898,7 +6862,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>184</v>
       </c>
@@ -6915,7 +6879,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -6932,7 +6896,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>187</v>
       </c>
@@ -6949,7 +6913,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -6966,7 +6930,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -6983,7 +6947,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -7000,7 +6964,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -7017,7 +6981,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -7034,7 +6998,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>66</v>
       </c>
@@ -7051,7 +7015,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>67</v>
       </c>
@@ -7068,7 +7032,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>68</v>
       </c>
@@ -7085,7 +7049,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>69</v>
       </c>
@@ -7102,7 +7066,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>140</v>
       </c>
@@ -7119,7 +7083,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>77</v>
       </c>
@@ -7136,7 +7100,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>78</v>
       </c>
@@ -7153,7 +7117,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>79</v>
       </c>
@@ -7170,7 +7134,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>80</v>
       </c>
@@ -7187,7 +7151,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>81</v>
       </c>
@@ -7204,7 +7168,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>82</v>
       </c>
@@ -7221,7 +7185,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>83</v>
       </c>
@@ -7235,7 +7199,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>84</v>
       </c>
@@ -7249,7 +7213,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>85</v>
       </c>
@@ -7263,7 +7227,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>89</v>
       </c>
@@ -7277,7 +7241,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>88</v>
       </c>
@@ -7291,7 +7255,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>86</v>
       </c>
@@ -7305,7 +7269,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>87</v>
       </c>
@@ -7319,7 +7283,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>242</v>
       </c>
@@ -7336,7 +7300,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>243</v>
       </c>
@@ -7353,7 +7317,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>95</v>
       </c>
@@ -7370,7 +7334,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>96</v>
       </c>
@@ -7387,7 +7351,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>97</v>
       </c>
@@ -7404,7 +7368,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>98</v>
       </c>
@@ -7421,7 +7385,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>107</v>
       </c>
@@ -7435,7 +7399,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>108</v>
       </c>
@@ -7449,7 +7413,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>109</v>
       </c>
@@ -7463,7 +7427,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>110</v>
       </c>
@@ -7477,7 +7441,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>114</v>
       </c>
@@ -7491,7 +7455,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>142</v>
       </c>
@@ -7508,7 +7472,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>145</v>
       </c>
@@ -7525,7 +7489,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>148</v>
       </c>
@@ -7542,7 +7506,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>149</v>
       </c>
@@ -7559,7 +7523,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>150</v>
       </c>
@@ -7573,7 +7537,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>151</v>
       </c>
@@ -7588,7 +7552,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>152</v>
       </c>
@@ -7603,7 +7567,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>153</v>
       </c>
@@ -7618,7 +7582,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>192</v>
       </c>
@@ -7635,7 +7599,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>191</v>
       </c>
@@ -7652,7 +7616,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
         <v>229</v>
       </c>
@@ -7666,7 +7630,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="9" t="s">
         <v>230</v>
       </c>
@@ -7680,7 +7644,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="9" t="s">
         <v>231</v>
       </c>
@@ -7694,7 +7658,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>17</v>
       </c>
@@ -7711,7 +7675,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>15</v>
       </c>
@@ -7728,7 +7692,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>12</v>
       </c>
@@ -7742,7 +7706,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>73</v>
       </c>
@@ -7756,7 +7720,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>211</v>
       </c>

</xml_diff>

<commit_message>
Key change: updated the SpeciesDefinitionFile.xlsx to reflect the latest values for survival reduction for the pelagic feeding ecology groups survival reduction. See see CARMMHA\integrativemodelling\ModelComponents\1 Expert Elicitation Outputs\SurvivalFactorUpdate2022\SurvivalFraction_v2_TAM.pdf for details, old values and values now considered.
</commit_message>
<xml_diff>
--- a/FolderArchitecture2runCode/InputFiles/SpeciesDefinitionFile.xlsx
+++ b/FolderArchitecture2runCode/InputFiles/SpeciesDefinitionFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tam2\Dropbox\Trabalho\Funded\CARMMHA\integrativemodelling\FinalModelRuns\CARMMHAgit\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915BFF65-861F-4CE0-9848-52D4D26045CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F523688-460D-4051-A6CE-BED60A4B7CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29940" yWindow="1140" windowWidth="21600" windowHeight="11265" tabRatio="930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51720" yWindow="-3015" windowWidth="51840" windowHeight="21240" tabRatio="930" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="values" sheetId="32" r:id="rId1"/>
@@ -71,7 +71,7 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    will come from Richard's analysis</t>
+    now comes from Richard's analysis</t>
       </text>
     </comment>
     <comment ref="AO25" authorId="4" shapeId="0" xr:uid="{9555694C-6EFE-4219-8D3C-BBE6F63D7731}">
@@ -851,13 +851,13 @@
     <t>Color code - note to all: never use color codes in Excel, but rules are made to be broken :) - dark green is a stock in offshore paper, light green is the BB population;</t>
   </si>
   <si>
-    <t>used for non-BB BND only</t>
-  </si>
-  <si>
     <t>standard deviation of successes for baseline reproductive success. Superseeds suc4brs</t>
   </si>
   <si>
     <t>standard deviation for post oil spill reproductive success. Superseeds suc4pors</t>
+  </si>
+  <si>
+    <t>used for non-BB BND only. Color coded with conditional formatting for the 3 different feeding ecology groups - see CARMMHA\integrativemodelling\ModelComponents\1 Expert Elicitation Outputs\SurvivalFactorUpdate2022\SurvivalFraction_v2_TAM.pdf</t>
   </si>
 </sst>
 </file>
@@ -1631,7 +1631,469 @@
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Warning Text 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="76">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -2084,7 +2546,7 @@
     <text>value changed from 0.34 on the 21st April 2021. See email from Len Mon 4/19/2021 12:15 AM replying to Lori (Sun 4/18/2021 10:18 PM)</text>
   </threadedComment>
   <threadedComment ref="AA25" dT="2020-05-27T16:17:04.72" personId="{43E54F80-8E8C-427E-A997-6277C6651A43}" id="{FBDD81FD-7A18-4735-8879-CB35D02C7391}">
-    <text>will come from Richard's analysis</text>
+    <text>now comes from Richard's analysis</text>
   </threadedComment>
   <threadedComment ref="AO25" dT="2020-06-15T14:57:08.01" personId="{43E54F80-8E8C-427E-A997-6277C6651A43}" id="{9555694C-6EFE-4219-8D3C-BBE6F63D7731}">
     <text>Decision reached by consensus on phone call the 15th June 2020</text>
@@ -2099,11 +2561,11 @@
   </sheetPr>
   <dimension ref="A1:BG34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AN2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AZ38" sqref="AZ38"/>
+      <selection pane="bottomRight" activeCell="AF45" sqref="AF45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2572,16 +3034,16 @@
         <v>1.1723330000000001</v>
       </c>
       <c r="AA3" s="3">
-        <v>0.63</v>
+        <v>0.52600000000000002</v>
       </c>
       <c r="AB3" s="3">
         <v>0.99</v>
       </c>
       <c r="AC3" s="3">
-        <v>4.16</v>
+        <v>3.3490000000000002</v>
       </c>
       <c r="AD3" s="3">
-        <v>2.96</v>
+        <v>1.992</v>
       </c>
       <c r="AE3" s="3" t="s">
         <v>94</v>
@@ -2748,16 +3210,16 @@
         <v>1.1723330000000001</v>
       </c>
       <c r="AA4" s="3">
-        <v>0.7</v>
+        <v>0.59399999999999997</v>
       </c>
       <c r="AB4" s="3">
         <v>0.99</v>
       </c>
       <c r="AC4" s="3">
-        <v>4.18</v>
+        <v>3.4990000000000001</v>
       </c>
       <c r="AD4" s="3">
-        <v>3.61</v>
+        <v>2.23</v>
       </c>
       <c r="AE4" s="3" t="s">
         <v>94</v>
@@ -2924,16 +3386,16 @@
         <v>1.1723330000000001</v>
       </c>
       <c r="AA5" s="3">
-        <v>0.7</v>
+        <v>0.59399999999999997</v>
       </c>
       <c r="AB5" s="3">
         <v>0.99</v>
       </c>
       <c r="AC5" s="3">
-        <v>4.18</v>
+        <v>3.4990000000000001</v>
       </c>
       <c r="AD5" s="3">
-        <v>3.61</v>
+        <v>2.23</v>
       </c>
       <c r="AE5" s="3" t="s">
         <v>94</v>
@@ -3100,16 +3562,16 @@
         <v>1.1723330000000001</v>
       </c>
       <c r="AA6" s="3">
-        <v>0.7</v>
+        <v>0.59399999999999997</v>
       </c>
       <c r="AB6" s="3">
         <v>0.99</v>
       </c>
       <c r="AC6" s="3">
-        <v>4.18</v>
+        <v>3.4990000000000001</v>
       </c>
       <c r="AD6" s="3">
-        <v>3.61</v>
+        <v>2.23</v>
       </c>
       <c r="AE6" s="3" t="s">
         <v>94</v>
@@ -3276,16 +3738,16 @@
         <v>1.1723330000000001</v>
       </c>
       <c r="AA7" s="4">
-        <v>0.7</v>
+        <v>0.59399999999999997</v>
       </c>
       <c r="AB7" s="4">
         <v>0.99</v>
       </c>
       <c r="AC7" s="4">
-        <v>4.18</v>
+        <v>3.4990000000000001</v>
       </c>
       <c r="AD7" s="4">
-        <v>3.61</v>
+        <v>2.23</v>
       </c>
       <c r="AE7" s="3" t="s">
         <v>94</v>
@@ -3455,16 +3917,16 @@
         <v>1.1723330000000001</v>
       </c>
       <c r="AA8" s="4">
-        <v>0.7</v>
+        <v>0.59399999999999997</v>
       </c>
       <c r="AB8" s="4">
         <v>0.99</v>
       </c>
       <c r="AC8" s="4">
-        <v>4.18</v>
+        <v>3.4990000000000001</v>
       </c>
       <c r="AD8" s="4">
-        <v>3.61</v>
+        <v>2.23</v>
       </c>
       <c r="AE8" s="3" t="s">
         <v>94</v>
@@ -3631,16 +4093,16 @@
         <v>1.1723330000000001</v>
       </c>
       <c r="AA9" s="4">
-        <v>0.7</v>
+        <v>0.59399999999999997</v>
       </c>
       <c r="AB9" s="4">
         <v>0.99</v>
       </c>
       <c r="AC9" s="4">
-        <v>4.18</v>
+        <v>3.4990000000000001</v>
       </c>
       <c r="AD9" s="4">
-        <v>3.61</v>
+        <v>2.23</v>
       </c>
       <c r="AE9" s="3" t="s">
         <v>94</v>
@@ -3810,16 +4272,16 @@
         <v>1.1723330000000001</v>
       </c>
       <c r="AA10" s="3">
-        <v>0.75</v>
+        <v>0.63700000000000001</v>
       </c>
       <c r="AB10" s="3">
         <v>0.99</v>
       </c>
       <c r="AC10" s="3">
-        <v>4.3704390000000002</v>
+        <v>3.5150000000000001</v>
       </c>
       <c r="AD10" s="3">
-        <v>3.5804640000000001</v>
+        <v>2.016</v>
       </c>
       <c r="AE10" s="3" t="s">
         <v>94</v>
@@ -3989,16 +4451,16 @@
         <v>1.1723330000000001</v>
       </c>
       <c r="AA11" s="3">
-        <v>0.63</v>
+        <v>0.52600000000000002</v>
       </c>
       <c r="AB11" s="3">
         <v>0.99</v>
       </c>
       <c r="AC11" s="3">
-        <v>4.16</v>
+        <v>3.3490000000000002</v>
       </c>
       <c r="AD11" s="3">
-        <v>2.96</v>
+        <v>1.992</v>
       </c>
       <c r="AE11" s="3" t="s">
         <v>94</v>
@@ -4168,16 +4630,16 @@
         <v>1.1723330000000001</v>
       </c>
       <c r="AA12" s="3">
-        <v>0.63</v>
+        <v>0.52600000000000002</v>
       </c>
       <c r="AB12" s="3">
         <v>0.99</v>
       </c>
       <c r="AC12" s="3">
-        <v>4.16</v>
+        <v>3.3490000000000002</v>
       </c>
       <c r="AD12" s="3">
-        <v>2.96</v>
+        <v>1.992</v>
       </c>
       <c r="AE12" s="3" t="s">
         <v>94</v>
@@ -4347,16 +4809,16 @@
         <v>1.1723330000000001</v>
       </c>
       <c r="AA13" s="4">
-        <v>0.7</v>
+        <v>0.59399999999999997</v>
       </c>
       <c r="AB13" s="4">
         <v>0.99</v>
       </c>
       <c r="AC13" s="4">
-        <v>4.18</v>
+        <v>3.4990000000000001</v>
       </c>
       <c r="AD13" s="4">
-        <v>3.61</v>
+        <v>2.23</v>
       </c>
       <c r="AE13" s="3" t="s">
         <v>94</v>
@@ -4526,16 +4988,16 @@
         <v>1.1723330000000001</v>
       </c>
       <c r="AA14" s="4">
-        <v>0.7</v>
+        <v>0.59399999999999997</v>
       </c>
       <c r="AB14" s="4">
         <v>0.99</v>
       </c>
       <c r="AC14" s="4">
-        <v>4.18</v>
+        <v>3.4990000000000001</v>
       </c>
       <c r="AD14" s="4">
-        <v>3.61</v>
+        <v>2.23</v>
       </c>
       <c r="AE14" s="3" t="s">
         <v>94</v>
@@ -4702,16 +5164,16 @@
         <v>1.1723330000000001</v>
       </c>
       <c r="AA15" s="4">
-        <v>0.63</v>
+        <v>0.52600000000000002</v>
       </c>
       <c r="AB15" s="4">
         <v>0.99</v>
       </c>
       <c r="AC15" s="4">
-        <v>4.16</v>
+        <v>3.3490000000000002</v>
       </c>
       <c r="AD15" s="4">
-        <v>2.96</v>
+        <v>1.992</v>
       </c>
       <c r="AE15" s="3" t="s">
         <v>94</v>
@@ -4878,16 +5340,16 @@
         <v>1.1723330000000001</v>
       </c>
       <c r="AA16" s="3">
-        <v>0.75</v>
+        <v>0.63700000000000001</v>
       </c>
       <c r="AB16" s="3">
         <v>0.99</v>
       </c>
       <c r="AC16" s="3">
-        <v>4.3704390000000002</v>
+        <v>3.5150000000000001</v>
       </c>
       <c r="AD16" s="3">
-        <v>3.5804640000000001</v>
+        <v>2.016</v>
       </c>
       <c r="AE16" s="3" t="s">
         <v>94</v>
@@ -5054,16 +5516,16 @@
         <v>1.1723330000000001</v>
       </c>
       <c r="AA17" s="3">
-        <v>0.7</v>
+        <v>0.59399999999999997</v>
       </c>
       <c r="AB17" s="3">
         <v>0.99</v>
       </c>
       <c r="AC17" s="3">
-        <v>4.18</v>
+        <v>3.4990000000000001</v>
       </c>
       <c r="AD17" s="3">
-        <v>3.61</v>
+        <v>2.23</v>
       </c>
       <c r="AE17" s="3" t="s">
         <v>94</v>
@@ -5230,16 +5692,16 @@
         <v>1</v>
       </c>
       <c r="AA18" s="4">
-        <v>0.7</v>
+        <v>0.59399999999999997</v>
       </c>
       <c r="AB18" s="4">
         <v>0.99</v>
       </c>
       <c r="AC18" s="4">
-        <v>4.18</v>
+        <v>3.4990000000000001</v>
       </c>
       <c r="AD18" s="4">
-        <v>3.61</v>
+        <v>2.23</v>
       </c>
       <c r="AE18" s="4">
         <v>75.8</v>
@@ -5409,16 +5871,16 @@
         <v>1.1723330000000001</v>
       </c>
       <c r="AA19" s="4">
-        <v>0.75</v>
+        <v>0.63700000000000001</v>
       </c>
       <c r="AB19" s="4">
         <v>0.99</v>
       </c>
       <c r="AC19" s="4">
-        <v>4.3704390000000002</v>
+        <v>3.5150000000000001</v>
       </c>
       <c r="AD19" s="4">
-        <v>3.5804640000000001</v>
+        <v>2.016</v>
       </c>
       <c r="AE19" s="3" t="s">
         <v>94</v>
@@ -5585,16 +6047,16 @@
         <v>1.1723330000000001</v>
       </c>
       <c r="AA20" s="3">
-        <v>0.75</v>
+        <v>0.63700000000000001</v>
       </c>
       <c r="AB20" s="3">
         <v>0.99</v>
       </c>
       <c r="AC20" s="3">
-        <v>4.3704390000000002</v>
+        <v>3.5150000000000001</v>
       </c>
       <c r="AD20" s="3">
-        <v>3.5804640000000001</v>
+        <v>2.016</v>
       </c>
       <c r="AE20" s="3" t="s">
         <v>94</v>
@@ -5761,16 +6223,16 @@
         <v>1.1723330000000001</v>
       </c>
       <c r="AA21" s="3">
-        <v>0.75</v>
+        <v>0.63700000000000001</v>
       </c>
       <c r="AB21" s="3">
         <v>0.99</v>
       </c>
       <c r="AC21" s="3">
-        <v>4.3704390000000002</v>
+        <v>3.5150000000000001</v>
       </c>
       <c r="AD21" s="3">
-        <v>3.5804640000000001</v>
+        <v>2.016</v>
       </c>
       <c r="AE21" s="3" t="s">
         <v>94</v>
@@ -5937,16 +6399,16 @@
         <v>1.1723330000000001</v>
       </c>
       <c r="AA22" s="3">
-        <v>0.75</v>
+        <v>0.63700000000000001</v>
       </c>
       <c r="AB22" s="3">
         <v>0.99</v>
       </c>
       <c r="AC22" s="3">
-        <v>4.3704390000000002</v>
+        <v>3.5150000000000001</v>
       </c>
       <c r="AD22" s="3">
-        <v>3.5804640000000001</v>
+        <v>2.016</v>
       </c>
       <c r="AE22" s="3" t="s">
         <v>94</v>
@@ -6113,16 +6575,16 @@
         <v>1.1723330000000001</v>
       </c>
       <c r="AA23" s="4">
-        <v>0.7</v>
+        <v>0.59399999999999997</v>
       </c>
       <c r="AB23" s="4">
         <v>0.99</v>
       </c>
       <c r="AC23" s="4">
-        <v>4.18</v>
+        <v>3.4990000000000001</v>
       </c>
       <c r="AD23" s="4">
-        <v>3.61</v>
+        <v>2.23</v>
       </c>
       <c r="AE23" s="3" t="s">
         <v>94</v>
@@ -6289,16 +6751,16 @@
         <v>1.1723330000000001</v>
       </c>
       <c r="AA24" s="3">
-        <v>0.75</v>
+        <v>0.63700000000000001</v>
       </c>
       <c r="AB24" s="3">
         <v>0.99</v>
       </c>
       <c r="AC24" s="3">
-        <v>4.3704390000000002</v>
+        <v>3.5150000000000001</v>
       </c>
       <c r="AD24" s="3">
-        <v>3.5804640000000001</v>
+        <v>2.016</v>
       </c>
       <c r="AE24" s="3" t="s">
         <v>94</v>
@@ -6464,16 +6926,16 @@
       <c r="Z25" s="1">
         <v>1.1723330000000001</v>
       </c>
-      <c r="AA25" s="7">
+      <c r="AA25" s="4">
         <v>0.7</v>
       </c>
-      <c r="AB25" s="7">
+      <c r="AB25" s="4">
         <v>0.99</v>
       </c>
-      <c r="AC25" s="7">
+      <c r="AC25" s="4">
         <v>4.18</v>
       </c>
-      <c r="AD25" s="7">
+      <c r="AD25" s="4">
         <v>3.61</v>
       </c>
       <c r="AE25" s="4">
@@ -6641,16 +7103,16 @@
         <v>1.1723330000000001</v>
       </c>
       <c r="AA26" s="3">
-        <v>0.63</v>
+        <v>0.52600000000000002</v>
       </c>
       <c r="AB26" s="3">
         <v>0.99</v>
       </c>
       <c r="AC26" s="3">
-        <v>4.16</v>
+        <v>3.3490000000000002</v>
       </c>
       <c r="AD26" s="3">
-        <v>2.96</v>
+        <v>1.992</v>
       </c>
       <c r="AE26" s="3" t="s">
         <v>94</v>
@@ -6774,6 +7236,45 @@
     <sortCondition ref="A2:A34"/>
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
+  <conditionalFormatting sqref="AA1:AA1048576">
+    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
+      <formula>0.637</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
+      <formula>0.594</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
+      <formula>0.526</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC1:AC1048576">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
+      <formula>3.439</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
+      <formula>3.349</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+      <formula>3.499</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+      <formula>3.515</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD1:AD1048576">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+      <formula>1.992</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+      <formula>3.499</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>2.23</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>2.016</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -6784,8 +7285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899DABE4-7FD8-4E75-8254-AD3B5E1176D5}">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7261,7 +7762,7 @@
         <v>93</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -7278,7 +7779,7 @@
         <v>93</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -7295,7 +7796,7 @@
         <v>93</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -7312,7 +7813,7 @@
         <v>93</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -7577,7 +8078,7 @@
         <v>151</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>124</v>
@@ -7607,7 +8108,7 @@
         <v>153</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>124</v>
@@ -7772,42 +8273,42 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="C2:C50 C53:C60">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Deprecated">
+    <cfRule type="containsText" dxfId="75" priority="9" operator="containsText" text="Deprecated">
       <formula>NOT(ISERROR(SEARCH("Deprecated",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Active">
+    <cfRule type="containsText" dxfId="74" priority="10" operator="containsText" text="Active">
       <formula>NOT(ISERROR(SEARCH("Active",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56:E57 E47:E50 D1:D50 D53:D1048576 E28:E33">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Expert">
+    <cfRule type="containsText" dxfId="73" priority="7" operator="containsText" text="Expert">
       <formula>NOT(ISERROR(SEARCH("Expert",D1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="8" operator="equal">
       <formula>"Expert"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:E24">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Expert">
+    <cfRule type="containsText" dxfId="71" priority="5" operator="containsText" text="Expert">
       <formula>NOT(ISERROR(SEARCH("Expert",E19)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="6" operator="equal">
       <formula>"Expert"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51:C52">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Deprecated">
+    <cfRule type="containsText" dxfId="69" priority="3" operator="containsText" text="Deprecated">
       <formula>NOT(ISERROR(SEARCH("Deprecated",C51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Active">
+    <cfRule type="containsText" dxfId="68" priority="4" operator="containsText" text="Active">
       <formula>NOT(ISERROR(SEARCH("Active",C51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51:E52">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Expert">
+    <cfRule type="containsText" dxfId="67" priority="1" operator="containsText" text="Expert">
       <formula>NOT(ISERROR(SEARCH("Expert",D51)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="2" operator="equal">
       <formula>"Expert"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>